<commit_message>
Casi casi casi listo
</commit_message>
<xml_diff>
--- a/porticos/datos.xlsx
+++ b/porticos/datos.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Hoja 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -414,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -425,99 +424,1082 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Está imprimiendo LAJA</t>
+          <t>Usuario</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Fecha y Hora</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Cámara</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Infracción</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>En el rango de fecha 06-05-2024 y 09-05-2024</t>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>13/05/2024 15:02:20</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Registros globales</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>6173</v>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>13/05/2024 14:48:02</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Infracciones globales</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>13/05/2024 14:24:20</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Fallos globales</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>4597</v>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>13/05/2024 14:24:17</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>13/05/2024 13:05:21</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>13/05/2024 13:05:15</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>13/05/2024 13:02:12</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>13/05/2024 10:44:06</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>13/05/2024 09:36:14</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>13/05/2024 08:37:46</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>13/05/2024 07:01:22</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>11/05/2024 15:51:04</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>11/05/2024 15:50:59</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>11/05/2024 11:22:54</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>11/05/2024 11:15:24</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>11/05/2024 10:27:59</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>11/05/2024 09:50:58</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>11/05/2024 09:32:02</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>11/05/2024 08:36:40</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>11/05/2024 08:17:43</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>11/05/2024 08:17:39</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>10/05/2024 13:52:33</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>10/05/2024 11:31:36</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>10/05/2024 10:28:34</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>09/05/2024 18:10:13</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N2</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>09/05/2024 17:47:21</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>09/05/2024 14:01:19</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>09/05/2024 13:11:42</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>09/05/2024 12:41:04</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>08/05/2024 19:38:33</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>08/05/2024 18:41:55</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>08/05/2024 17:40:20</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>08/05/2024 17:16:14</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>08/05/2024 14:49:07</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>08/05/2024 14:20:25</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>08/05/2024 14:09:11</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>08/05/2024 12:58:12</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>08/05/2024 12:58:07</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>08/05/2024 12:18:06</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>08/05/2024 11:49:01</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>08/05/2024 11:29:34</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>08/05/2024 10:54:59</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>07/05/2024 20:31:07</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>07/05/2024 20:31:03</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>07/05/2024 15:18:36</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>07/05/2024 14:51:01</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>07/05/2024 10:21:43</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE S2</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>laja</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>07/05/2024 10:21:38</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ACCESO NORTE N1</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>LIMPIA</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Está imprimiendo LAJA</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>En el rango de fecha 06-05-2024 y 09-05-2024</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Hola</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>123</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>